<commit_message>
Arreglo de performance con conversion lazy a mapa
</commit_message>
<xml_diff>
--- a/Documentacion/drafts/20120630/Comparacion de velocidad con mensje modelo.xlsx
+++ b/Documentacion/drafts/20120630/Comparacion de velocidad con mensje modelo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="28635" windowHeight="12780" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="28635" windowHeight="12780"/>
   </bookViews>
   <sheets>
     <sheet name="26-05-2012" sheetId="2" r:id="rId1"/>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:J62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:J14"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1764,25 +1764,25 @@
         <v>41</v>
       </c>
       <c r="E53">
-        <v>10000</v>
+        <v>12781</v>
       </c>
       <c r="F53" s="1">
-        <v>22.635682907348201</v>
+        <v>29.180267584696001</v>
       </c>
       <c r="G53" s="1">
-        <v>21.124800319488799</v>
+        <v>1.2486503403489499</v>
       </c>
       <c r="H53" s="4">
         <f t="shared" ref="H53:H62" si="10">G53/F53</f>
-        <v>0.93325217560063423</v>
-      </c>
-      <c r="I53" s="5">
+        <v>4.2790914672894295E-2</v>
+      </c>
+      <c r="I53" s="6">
         <f>F53*1000</f>
-        <v>22635.6829073482</v>
-      </c>
-      <c r="J53" s="5">
+        <v>29180.267584696001</v>
+      </c>
+      <c r="J53" s="7">
         <f t="shared" ref="J53:J62" si="11">G53*1000</f>
-        <v>21124.800319488797</v>
+        <v>1248.6503403489498</v>
       </c>
     </row>
     <row r="54" spans="4:10" x14ac:dyDescent="0.25">
@@ -1790,25 +1790,25 @@
         <v>42</v>
       </c>
       <c r="E54">
-        <v>10938</v>
+        <v>10172</v>
       </c>
       <c r="F54" s="1">
-        <v>18.335618943134001</v>
+        <v>36.067046795123801</v>
       </c>
       <c r="G54" s="1">
-        <v>7.3678003291278102</v>
+        <v>3.1804954777821401</v>
       </c>
       <c r="H54" s="4">
         <f t="shared" si="10"/>
-        <v>0.40182992196654338</v>
+        <v>8.8182863871519898E-2</v>
       </c>
       <c r="I54" s="7">
         <f t="shared" ref="I54:I62" si="12">F54*1000</f>
-        <v>18335.618943134003</v>
+        <v>36067.046795123802</v>
       </c>
       <c r="J54" s="7">
         <f t="shared" si="11"/>
-        <v>7367.8003291278101</v>
+        <v>3180.4954777821404</v>
       </c>
     </row>
     <row r="55" spans="4:10" x14ac:dyDescent="0.25">
@@ -1816,25 +1816,25 @@
         <v>43</v>
       </c>
       <c r="E55">
-        <v>11688</v>
+        <v>10375</v>
       </c>
       <c r="F55" s="1">
-        <v>17.152464065708401</v>
+        <v>36.081734939759002</v>
       </c>
       <c r="G55" s="1">
-        <v>4.2945756331279901</v>
+        <v>5.8360481927710799</v>
       </c>
       <c r="H55" s="4">
         <f t="shared" si="10"/>
-        <v>0.25037659992617645</v>
+        <v>0.16174522102428759</v>
       </c>
       <c r="I55" s="7">
         <f t="shared" si="12"/>
-        <v>17152.464065708402</v>
+        <v>36081.734939759001</v>
       </c>
       <c r="J55" s="7">
         <f t="shared" si="11"/>
-        <v>4294.5756331279899</v>
+        <v>5836.0481927710798</v>
       </c>
     </row>
     <row r="56" spans="4:10" x14ac:dyDescent="0.25">
@@ -1842,25 +1842,25 @@
         <v>44</v>
       </c>
       <c r="E56">
-        <v>10125</v>
+        <v>10766</v>
       </c>
       <c r="F56" s="1">
-        <v>18.6720987654321</v>
+        <v>33.577651866988603</v>
       </c>
       <c r="G56" s="1">
-        <v>1.46646913580246</v>
+        <v>5.4699981422998301</v>
       </c>
       <c r="H56" s="4">
         <f t="shared" si="10"/>
-        <v>7.8537991589748515E-2</v>
+        <v>0.16290591623167019</v>
       </c>
       <c r="I56" s="7">
         <f t="shared" si="12"/>
-        <v>18672.0987654321</v>
+        <v>33577.651866988606</v>
       </c>
       <c r="J56" s="7">
         <f t="shared" si="11"/>
-        <v>1466.46913580246</v>
+        <v>5469.9981422998299</v>
       </c>
     </row>
     <row r="57" spans="4:10" x14ac:dyDescent="0.25">
@@ -1868,25 +1868,25 @@
         <v>45</v>
       </c>
       <c r="E57">
-        <v>11172</v>
+        <v>11515</v>
       </c>
       <c r="F57" s="1">
-        <v>17.222162549230202</v>
+        <v>31.925835866261298</v>
       </c>
       <c r="G57" s="1">
-        <v>0.73182957393483705</v>
+        <v>1.3814155449413801</v>
       </c>
       <c r="H57" s="4">
         <f t="shared" si="10"/>
-        <v>4.2493477334386701E-2</v>
+        <v>4.3269518478018534E-2</v>
       </c>
       <c r="I57" s="7">
         <f t="shared" si="12"/>
-        <v>17222.162549230201</v>
-      </c>
-      <c r="J57" s="6">
+        <v>31925.835866261299</v>
+      </c>
+      <c r="J57" s="7">
         <f t="shared" si="11"/>
-        <v>731.82957393483707</v>
+        <v>1381.4155449413802</v>
       </c>
     </row>
     <row r="58" spans="4:10" x14ac:dyDescent="0.25">
@@ -1894,25 +1894,25 @@
         <v>46</v>
       </c>
       <c r="E58">
-        <v>12687</v>
+        <v>12031</v>
       </c>
       <c r="F58" s="1">
-        <v>16.317884448648201</v>
+        <v>31.350843653894099</v>
       </c>
       <c r="G58" s="1">
-        <v>0.77260187593599705</v>
+        <v>0.60502036405951198</v>
       </c>
       <c r="H58" s="4">
         <f t="shared" si="10"/>
-        <v>4.7346938775510244E-2</v>
+        <v>1.9298375850385199E-2</v>
       </c>
       <c r="I58" s="7">
         <f t="shared" si="12"/>
-        <v>16317.884448648201</v>
-      </c>
-      <c r="J58" s="7">
+        <v>31350.843653894099</v>
+      </c>
+      <c r="J58" s="6">
         <f t="shared" si="11"/>
-        <v>772.6018759359971</v>
+        <v>605.02036405951196</v>
       </c>
     </row>
     <row r="59" spans="4:10" x14ac:dyDescent="0.25">
@@ -1920,25 +1920,25 @@
         <v>47</v>
       </c>
       <c r="E59">
-        <v>10766</v>
+        <v>10063</v>
       </c>
       <c r="F59" s="1">
-        <v>20.394761285528499</v>
+        <v>36.818344430090399</v>
       </c>
       <c r="G59" s="1">
-        <v>2.1279955415195899</v>
+        <v>0.68418960548544105</v>
       </c>
       <c r="H59" s="4">
         <f t="shared" si="10"/>
-        <v>0.10434030149838286</v>
+        <v>1.8582845483032524E-2</v>
       </c>
       <c r="I59" s="7">
         <f t="shared" si="12"/>
-        <v>20394.761285528501</v>
+        <v>36818.344430090401</v>
       </c>
       <c r="J59" s="7">
         <f t="shared" si="11"/>
-        <v>2127.99554151959</v>
+        <v>684.18960548544101</v>
       </c>
     </row>
     <row r="60" spans="4:10" x14ac:dyDescent="0.25">
@@ -1946,25 +1946,25 @@
         <v>48</v>
       </c>
       <c r="E60">
-        <v>11187</v>
+        <v>10000</v>
       </c>
       <c r="F60" s="1">
-        <v>15.744614284437199</v>
+        <v>39.307000000000002</v>
       </c>
       <c r="G60" s="1">
-        <v>6.5506391347099298</v>
+        <v>2.7025000000000001</v>
       </c>
       <c r="H60" s="4">
         <f t="shared" si="10"/>
-        <v>0.41605586623896684</v>
-      </c>
-      <c r="I60" s="7">
+        <v>6.8753657109420718E-2</v>
+      </c>
+      <c r="I60" s="5">
         <f t="shared" si="12"/>
-        <v>15744.614284437199</v>
+        <v>39307</v>
       </c>
       <c r="J60" s="7">
         <f t="shared" si="11"/>
-        <v>6550.6391347099297</v>
+        <v>2702.5</v>
       </c>
     </row>
     <row r="61" spans="4:10" x14ac:dyDescent="0.25">
@@ -1972,25 +1972,25 @@
         <v>49</v>
       </c>
       <c r="E61">
-        <v>10860</v>
+        <v>11907</v>
       </c>
       <c r="F61" s="1">
-        <v>21.102025782688699</v>
+        <v>32.582514487276299</v>
       </c>
       <c r="G61" s="1">
-        <v>6.19861878453038</v>
+        <v>1.8858654572940201</v>
       </c>
       <c r="H61" s="4">
         <f t="shared" si="10"/>
-        <v>0.2937452000279277</v>
+        <v>5.7879678317352204E-2</v>
       </c>
       <c r="I61" s="7">
         <f t="shared" si="12"/>
-        <v>21102.025782688699</v>
+        <v>32582.514487276298</v>
       </c>
       <c r="J61" s="7">
         <f t="shared" si="11"/>
-        <v>6198.6187845303803</v>
+        <v>1885.8654572940202</v>
       </c>
     </row>
     <row r="62" spans="4:10" x14ac:dyDescent="0.25">
@@ -1998,25 +1998,25 @@
         <v>50</v>
       </c>
       <c r="E62">
-        <v>12641</v>
+        <v>11016</v>
       </c>
       <c r="F62" s="1">
-        <v>14.158452654062099</v>
+        <v>31.725671750181501</v>
       </c>
       <c r="G62" s="1">
-        <v>2.2265643540859101</v>
+        <v>6.4508896151053001</v>
       </c>
       <c r="H62" s="4">
         <f t="shared" si="10"/>
-        <v>0.15726043011113242</v>
-      </c>
-      <c r="I62" s="6">
+        <v>0.20333342871040688</v>
+      </c>
+      <c r="I62" s="7">
         <f t="shared" si="12"/>
-        <v>14158.452654062099</v>
-      </c>
-      <c r="J62" s="7">
+        <v>31725.6717501815</v>
+      </c>
+      <c r="J62" s="5">
         <f t="shared" si="11"/>
-        <v>2226.5643540859101</v>
+        <v>6450.8896151053004</v>
       </c>
     </row>
   </sheetData>
@@ -2280,8 +2280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Resultados de los tests volcados
</commit_message>
<xml_diff>
--- a/Documentacion/drafts/20120630/Comparacion de velocidad con mensje modelo.xlsx
+++ b/Documentacion/drafts/20120630/Comparacion de velocidad con mensje modelo.xlsx
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,22 +1496,22 @@
         <v>10000</v>
       </c>
       <c r="F41" s="1">
-        <v>41.873399999999997</v>
+        <v>42.019199999999998</v>
       </c>
       <c r="G41" s="1">
-        <v>30.869700000000002</v>
+        <v>35.879100000000001</v>
       </c>
       <c r="H41" s="4">
         <f t="shared" ref="H41:H50" si="8">G41/F41</f>
-        <v>0.73721503388786214</v>
+        <v>0.8538739433401874</v>
       </c>
       <c r="I41" s="7">
         <f>F41*1000</f>
-        <v>41873.399999999994</v>
+        <v>42019.199999999997</v>
       </c>
       <c r="J41" s="7">
         <f t="shared" si="1"/>
-        <v>30869.7</v>
+        <v>35879.1</v>
       </c>
     </row>
     <row r="42" spans="4:10" x14ac:dyDescent="0.25">
@@ -1519,25 +1519,25 @@
         <v>27</v>
       </c>
       <c r="E42">
-        <v>10078</v>
+        <v>10000</v>
       </c>
       <c r="F42" s="1">
-        <v>50.235860289740003</v>
+        <v>46.108600000000003</v>
       </c>
       <c r="G42" s="1">
-        <v>25.076800952569901</v>
+        <v>29.967700000000001</v>
       </c>
       <c r="H42" s="4">
         <f t="shared" si="8"/>
-        <v>0.4991812782330613</v>
-      </c>
-      <c r="I42" s="5">
+        <v>0.64993732188789077</v>
+      </c>
+      <c r="I42" s="7">
         <f t="shared" ref="I42:I50" si="9">F42*1000</f>
-        <v>50235.860289740005</v>
+        <v>46108.600000000006</v>
       </c>
       <c r="J42" s="7">
         <f t="shared" si="1"/>
-        <v>25076.800952569902</v>
+        <v>29967.7</v>
       </c>
     </row>
     <row r="43" spans="4:10" x14ac:dyDescent="0.25">
@@ -1545,25 +1545,25 @@
         <v>28</v>
       </c>
       <c r="E43">
-        <v>10437</v>
+        <v>10266</v>
       </c>
       <c r="F43" s="1">
-        <v>42.333045894414099</v>
+        <v>43.327586206896498</v>
       </c>
       <c r="G43" s="1">
-        <v>3.7998466992430702</v>
+        <v>4.1697837521916998</v>
       </c>
       <c r="H43" s="4">
         <f t="shared" si="8"/>
-        <v>8.9760767716089734E-2</v>
+        <v>9.6238542629175847E-2</v>
       </c>
       <c r="I43" s="7">
         <f t="shared" si="9"/>
-        <v>42333.045894414099</v>
-      </c>
-      <c r="J43" s="6">
-        <f t="shared" si="1"/>
-        <v>3799.8466992430704</v>
+        <v>43327.5862068965</v>
+      </c>
+      <c r="J43" s="7">
+        <f t="shared" si="1"/>
+        <v>4169.7837521916999</v>
       </c>
     </row>
     <row r="44" spans="4:10" x14ac:dyDescent="0.25">
@@ -1571,25 +1571,25 @@
         <v>29</v>
       </c>
       <c r="E44">
-        <v>10000</v>
+        <v>10032</v>
       </c>
       <c r="F44" s="1">
-        <v>48.076500000000003</v>
+        <v>50.854964114832498</v>
       </c>
       <c r="G44" s="1">
-        <v>11.223100000000001</v>
+        <v>19.509968102073302</v>
       </c>
       <c r="H44" s="4">
         <f t="shared" si="8"/>
-        <v>0.23344253429430178</v>
-      </c>
-      <c r="I44" s="7">
+        <v>0.38363940357954102</v>
+      </c>
+      <c r="I44" s="5">
         <f t="shared" si="9"/>
-        <v>48076.5</v>
+        <v>50854.964114832495</v>
       </c>
       <c r="J44" s="7">
         <f t="shared" si="1"/>
-        <v>11223.1</v>
+        <v>19509.968102073301</v>
       </c>
     </row>
     <row r="45" spans="4:10" x14ac:dyDescent="0.25">
@@ -1597,25 +1597,25 @@
         <v>30</v>
       </c>
       <c r="E45">
-        <v>10109</v>
+        <v>10000</v>
       </c>
       <c r="F45" s="1">
-        <v>49.815906617865203</v>
+        <v>44.218699999999998</v>
       </c>
       <c r="G45" s="1">
-        <v>44.106538727866202</v>
+        <v>41.266399999999997</v>
       </c>
       <c r="H45" s="4">
         <f t="shared" si="8"/>
-        <v>0.88539066580088133</v>
+        <v>0.93323412945201911</v>
       </c>
       <c r="I45" s="7">
         <f t="shared" si="9"/>
-        <v>49815.906617865199</v>
+        <v>44218.7</v>
       </c>
       <c r="J45" s="5">
         <f t="shared" si="1"/>
-        <v>44106.538727866202</v>
+        <v>41266.399999999994</v>
       </c>
     </row>
     <row r="46" spans="4:10" x14ac:dyDescent="0.25">
@@ -1623,25 +1623,25 @@
         <v>31</v>
       </c>
       <c r="E46">
-        <v>10344</v>
+        <v>10594</v>
       </c>
       <c r="F46" s="1">
-        <v>37.579369682907902</v>
+        <v>37.8011138380215</v>
       </c>
       <c r="G46" s="1">
-        <v>37.284706109822103</v>
+        <v>37.3301868982442</v>
       </c>
       <c r="H46" s="4">
         <f t="shared" si="8"/>
-        <v>0.99215890059966017</v>
+        <v>0.98754198244540548</v>
       </c>
       <c r="I46" s="7">
         <f t="shared" si="9"/>
-        <v>37579.369682907905</v>
+        <v>37801.113838021498</v>
       </c>
       <c r="J46" s="7">
         <f t="shared" si="1"/>
-        <v>37284.706109822102</v>
+        <v>37330.186898244203</v>
       </c>
     </row>
     <row r="47" spans="4:10" x14ac:dyDescent="0.25">
@@ -1649,25 +1649,25 @@
         <v>32</v>
       </c>
       <c r="E47">
-        <v>20172</v>
+        <v>24610</v>
       </c>
       <c r="F47" s="1">
-        <v>5.9030834820543303</v>
+        <v>5.9205607476635498</v>
       </c>
       <c r="G47" s="1">
-        <v>5.8185603807257502</v>
+        <v>5.8616822429906499</v>
       </c>
       <c r="H47" s="4">
         <f t="shared" si="8"/>
-        <v>0.98568153379745782</v>
+        <v>0.99005524861878402</v>
       </c>
       <c r="I47" s="6">
         <f t="shared" si="9"/>
-        <v>5903.0834820543305</v>
-      </c>
-      <c r="J47" s="7">
-        <f t="shared" si="1"/>
-        <v>5818.5603807257503</v>
+        <v>5920.5607476635496</v>
+      </c>
+      <c r="J47" s="6">
+        <f t="shared" si="1"/>
+        <v>5861.6822429906497</v>
       </c>
     </row>
     <row r="48" spans="4:10" x14ac:dyDescent="0.25">
@@ -1678,22 +1678,22 @@
         <v>10000</v>
       </c>
       <c r="F48" s="1">
-        <v>42.000900000000001</v>
+        <v>31.038900000000002</v>
       </c>
       <c r="G48" s="1">
-        <v>41.998800000000003</v>
+        <v>31.0383</v>
       </c>
       <c r="H48" s="4">
         <f t="shared" si="8"/>
-        <v>0.99995000107140564</v>
-      </c>
-      <c r="I48" s="3">
+        <v>0.99998066941805275</v>
+      </c>
+      <c r="I48" s="7">
         <f t="shared" si="9"/>
-        <v>42000.9</v>
+        <v>31038.9</v>
       </c>
       <c r="J48" s="7">
         <f t="shared" si="1"/>
-        <v>41998.8</v>
+        <v>31038.3</v>
       </c>
     </row>
     <row r="49" spans="4:10" x14ac:dyDescent="0.25">
@@ -1701,25 +1701,25 @@
         <v>34</v>
       </c>
       <c r="E49">
-        <v>10734</v>
+        <v>10359</v>
       </c>
       <c r="F49" s="1">
-        <v>49.423700391280001</v>
+        <v>48.923448209286597</v>
       </c>
       <c r="G49" s="1">
-        <v>23.794857462269398</v>
+        <v>23.067284486919501</v>
       </c>
       <c r="H49" s="4">
         <f t="shared" si="8"/>
-        <v>0.48144629547947831</v>
-      </c>
-      <c r="I49" s="3">
+        <v>0.47149751972185994</v>
+      </c>
+      <c r="I49" s="7">
         <f t="shared" si="9"/>
-        <v>49423.700391279999</v>
+        <v>48923.448209286595</v>
       </c>
       <c r="J49" s="7">
         <f t="shared" si="1"/>
-        <v>23794.8574622694</v>
+        <v>23067.2844869195</v>
       </c>
     </row>
     <row r="50" spans="4:10" x14ac:dyDescent="0.25">
@@ -1727,25 +1727,25 @@
         <v>35</v>
       </c>
       <c r="E50">
-        <v>10047</v>
+        <v>10031</v>
       </c>
       <c r="F50" s="1">
-        <v>40.7819249527222</v>
+        <v>32.799322101485302</v>
       </c>
       <c r="G50" s="1">
-        <v>37.051458146710402</v>
+        <v>32.5479015053334</v>
       </c>
       <c r="H50" s="4">
         <f t="shared" si="8"/>
-        <v>0.90852646582189378</v>
-      </c>
-      <c r="I50" s="3">
+        <v>0.99233457949606474</v>
+      </c>
+      <c r="I50" s="7">
         <f t="shared" si="9"/>
-        <v>40781.924952722198</v>
+        <v>32799.322101485304</v>
       </c>
       <c r="J50" s="7">
         <f t="shared" si="1"/>
-        <v>37051.4581467104</v>
+        <v>32547.901505333401</v>
       </c>
     </row>
     <row r="51" spans="4:10" x14ac:dyDescent="0.25">
@@ -1764,25 +1764,25 @@
         <v>41</v>
       </c>
       <c r="E53">
-        <v>10000</v>
+        <v>10016</v>
       </c>
       <c r="F53" s="1">
-        <v>24.638000000000002</v>
+        <v>24.299720447284301</v>
       </c>
       <c r="G53" s="1">
-        <v>24.546500000000002</v>
+        <v>24.276058306709199</v>
       </c>
       <c r="H53" s="4">
         <f t="shared" ref="H53:H62" si="10">G53/F53</f>
-        <v>0.99628622453121196</v>
+        <v>0.99902623815667202</v>
       </c>
       <c r="I53" s="7">
         <f>F53*1000</f>
-        <v>24638</v>
+        <v>24299.7204472843</v>
       </c>
       <c r="J53" s="7">
         <f t="shared" ref="J53:J62" si="11">G53*1000</f>
-        <v>24546.5</v>
+        <v>24276.058306709197</v>
       </c>
     </row>
     <row r="54" spans="4:10" x14ac:dyDescent="0.25">
@@ -1793,22 +1793,22 @@
         <v>10000</v>
       </c>
       <c r="F54" s="1">
-        <v>24.445</v>
+        <v>24.190200000000001</v>
       </c>
       <c r="G54" s="1">
-        <v>24.3507</v>
+        <v>24.161300000000001</v>
       </c>
       <c r="H54" s="4">
         <f t="shared" si="10"/>
-        <v>0.99614236040089998</v>
+        <v>0.99880530132036938</v>
       </c>
       <c r="I54" s="7">
         <f t="shared" ref="I54:I62" si="12">F54*1000</f>
-        <v>24445</v>
+        <v>24190.2</v>
       </c>
       <c r="J54" s="7">
         <f t="shared" si="11"/>
-        <v>24350.7</v>
+        <v>24161.3</v>
       </c>
     </row>
     <row r="55" spans="4:10" x14ac:dyDescent="0.25">
@@ -1819,22 +1819,22 @@
         <v>10000</v>
       </c>
       <c r="F55" s="1">
-        <v>25.284600000000001</v>
+        <v>24.487200000000001</v>
       </c>
       <c r="G55" s="1">
-        <v>25.1861</v>
+        <v>24.4605</v>
       </c>
       <c r="H55" s="4">
         <f t="shared" si="10"/>
-        <v>0.99610434810121573</v>
+        <v>0.99890963442124858</v>
       </c>
       <c r="I55" s="7">
         <f t="shared" si="12"/>
-        <v>25284.600000000002</v>
+        <v>24487.200000000001</v>
       </c>
       <c r="J55" s="7">
         <f t="shared" si="11"/>
-        <v>25186.1</v>
+        <v>24460.5</v>
       </c>
     </row>
     <row r="56" spans="4:10" x14ac:dyDescent="0.25">
@@ -1845,22 +1845,22 @@
         <v>10000</v>
       </c>
       <c r="F56" s="1">
-        <v>24.826899999999998</v>
+        <v>24.171700000000001</v>
       </c>
       <c r="G56" s="1">
-        <v>24.727799999999998</v>
+        <v>24.146799999999999</v>
       </c>
       <c r="H56" s="4">
         <f t="shared" si="10"/>
-        <v>0.99600836189778019</v>
+        <v>0.99896986972368507</v>
       </c>
       <c r="I56" s="7">
         <f t="shared" si="12"/>
-        <v>24826.899999999998</v>
+        <v>24171.7</v>
       </c>
       <c r="J56" s="7">
         <f t="shared" si="11"/>
-        <v>24727.8</v>
+        <v>24146.799999999999</v>
       </c>
     </row>
     <row r="57" spans="4:10" x14ac:dyDescent="0.25">
@@ -1871,22 +1871,22 @@
         <v>10000</v>
       </c>
       <c r="F57" s="1">
-        <v>24.5548</v>
+        <v>23.453399999999998</v>
       </c>
       <c r="G57" s="1">
-        <v>24.456399999999999</v>
+        <v>23.438800000000001</v>
       </c>
       <c r="H57" s="4">
         <f t="shared" si="10"/>
-        <v>0.99599263687751471</v>
+        <v>0.99937748897814394</v>
       </c>
       <c r="I57" s="7">
         <f t="shared" si="12"/>
-        <v>24554.799999999999</v>
+        <v>23453.399999999998</v>
       </c>
       <c r="J57" s="7">
         <f t="shared" si="11"/>
-        <v>24456.399999999998</v>
+        <v>23438.799999999999</v>
       </c>
     </row>
     <row r="58" spans="4:10" x14ac:dyDescent="0.25">
@@ -1897,22 +1897,22 @@
         <v>10000</v>
       </c>
       <c r="F58" s="1">
-        <v>23.931899999999999</v>
+        <v>22.456099999999999</v>
       </c>
       <c r="G58" s="1">
-        <v>23.843599999999999</v>
+        <v>22.4252</v>
       </c>
       <c r="H58" s="4">
         <f t="shared" si="10"/>
-        <v>0.99631036399115824</v>
+        <v>0.99862398190246748</v>
       </c>
       <c r="I58" s="7">
         <f t="shared" si="12"/>
-        <v>23931.899999999998</v>
+        <v>22456.1</v>
       </c>
       <c r="J58" s="7">
         <f t="shared" si="11"/>
-        <v>23843.599999999999</v>
+        <v>22425.200000000001</v>
       </c>
     </row>
     <row r="59" spans="4:10" x14ac:dyDescent="0.25">
@@ -1920,25 +1920,25 @@
         <v>47</v>
       </c>
       <c r="E59">
-        <v>10094</v>
+        <v>10078</v>
       </c>
       <c r="F59" s="1">
-        <v>19.126312660986699</v>
+        <v>2.9554475094264698</v>
       </c>
       <c r="G59" s="1">
-        <v>18.2869031107588</v>
+        <v>0.70043659456241303</v>
       </c>
       <c r="H59" s="4">
         <f t="shared" si="10"/>
-        <v>0.95611231683250153</v>
+        <v>0.23699848917240246</v>
       </c>
       <c r="I59" s="6">
         <f t="shared" si="12"/>
-        <v>19126.312660986699</v>
+        <v>2955.4475094264699</v>
       </c>
       <c r="J59" s="6">
         <f t="shared" si="11"/>
-        <v>18286.903110758802</v>
+        <v>700.43659456241301</v>
       </c>
     </row>
     <row r="60" spans="4:10" x14ac:dyDescent="0.25">
@@ -1949,22 +1949,22 @@
         <v>10000</v>
       </c>
       <c r="F60" s="1">
-        <v>25.057500000000001</v>
+        <v>24.8874</v>
       </c>
       <c r="G60" s="1">
-        <v>24.9617</v>
+        <v>24.8597</v>
       </c>
       <c r="H60" s="4">
         <f t="shared" si="10"/>
-        <v>0.9961767933752369</v>
+        <v>0.99888698698940026</v>
       </c>
       <c r="I60" s="7">
         <f t="shared" si="12"/>
-        <v>25057.5</v>
+        <v>24887.399999999998</v>
       </c>
       <c r="J60" s="7">
         <f t="shared" si="11"/>
-        <v>24961.7</v>
+        <v>24859.7</v>
       </c>
     </row>
     <row r="61" spans="4:10" x14ac:dyDescent="0.25">
@@ -1975,22 +1975,22 @@
         <v>10000</v>
       </c>
       <c r="F61" s="1">
-        <v>25.6783</v>
+        <v>24.096800000000002</v>
       </c>
       <c r="G61" s="1">
-        <v>25.583100000000002</v>
+        <v>24.072800000000001</v>
       </c>
       <c r="H61" s="4">
         <f t="shared" si="10"/>
-        <v>0.99629258946269816</v>
+        <v>0.99900401713090536</v>
       </c>
       <c r="I61" s="5">
         <f t="shared" si="12"/>
-        <v>25678.3</v>
+        <v>24096.800000000003</v>
       </c>
       <c r="J61" s="5">
         <f t="shared" si="11"/>
-        <v>25583.100000000002</v>
+        <v>24072.799999999999</v>
       </c>
     </row>
     <row r="62" spans="4:10" x14ac:dyDescent="0.25">
@@ -2001,22 +2001,22 @@
         <v>10000</v>
       </c>
       <c r="F62" s="1">
-        <v>25.116299999999999</v>
+        <v>24.1386</v>
       </c>
       <c r="G62" s="1">
-        <v>25.021000000000001</v>
+        <v>24.1084</v>
       </c>
       <c r="H62" s="4">
         <f t="shared" si="10"/>
-        <v>0.99620565131010541</v>
+        <v>0.99874889181642679</v>
       </c>
       <c r="I62" s="7">
         <f t="shared" si="12"/>
-        <v>25116.3</v>
+        <v>24138.6</v>
       </c>
       <c r="J62" s="7">
         <f t="shared" si="11"/>
-        <v>25021</v>
+        <v>24108.399999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregado de sincronización en operaciones de lectura
</commit_message>
<xml_diff>
--- a/Documentacion/drafts/20120630/Comparacion de velocidad con mensje modelo.xlsx
+++ b/Documentacion/drafts/20120630/Comparacion de velocidad con mensje modelo.xlsx
@@ -660,7 +660,7 @@
   <dimension ref="D2:J62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1764,25 +1764,25 @@
         <v>41</v>
       </c>
       <c r="E53">
-        <v>10016</v>
+        <v>10000</v>
       </c>
       <c r="F53" s="1">
-        <v>24.299720447284301</v>
+        <v>29.633800000000001</v>
       </c>
       <c r="G53" s="1">
-        <v>24.276058306709199</v>
+        <v>29.606300000000001</v>
       </c>
       <c r="H53" s="4">
         <f t="shared" ref="H53:H62" si="10">G53/F53</f>
-        <v>0.99902623815667202</v>
+        <v>0.9990720056152097</v>
       </c>
       <c r="I53" s="7">
         <f>F53*1000</f>
-        <v>24299.7204472843</v>
+        <v>29633.8</v>
       </c>
       <c r="J53" s="7">
         <f t="shared" ref="J53:J62" si="11">G53*1000</f>
-        <v>24276.058306709197</v>
+        <v>29606.3</v>
       </c>
     </row>
     <row r="54" spans="4:10" x14ac:dyDescent="0.25">
@@ -1793,22 +1793,22 @@
         <v>10000</v>
       </c>
       <c r="F54" s="1">
-        <v>24.190200000000001</v>
+        <v>29.637</v>
       </c>
       <c r="G54" s="1">
-        <v>24.161300000000001</v>
+        <v>29.609200000000001</v>
       </c>
       <c r="H54" s="4">
         <f t="shared" si="10"/>
-        <v>0.99880530132036938</v>
+        <v>0.99906198333164631</v>
       </c>
       <c r="I54" s="7">
         <f t="shared" ref="I54:I62" si="12">F54*1000</f>
-        <v>24190.2</v>
+        <v>29637</v>
       </c>
       <c r="J54" s="7">
         <f t="shared" si="11"/>
-        <v>24161.3</v>
+        <v>29609.200000000001</v>
       </c>
     </row>
     <row r="55" spans="4:10" x14ac:dyDescent="0.25">
@@ -1819,22 +1819,22 @@
         <v>10000</v>
       </c>
       <c r="F55" s="1">
-        <v>24.487200000000001</v>
+        <v>29.539100000000001</v>
       </c>
       <c r="G55" s="1">
-        <v>24.4605</v>
+        <v>29.508600000000001</v>
       </c>
       <c r="H55" s="4">
         <f t="shared" si="10"/>
-        <v>0.99890963442124858</v>
+        <v>0.99896747023436738</v>
       </c>
       <c r="I55" s="7">
         <f t="shared" si="12"/>
-        <v>24487.200000000001</v>
+        <v>29539.100000000002</v>
       </c>
       <c r="J55" s="7">
         <f t="shared" si="11"/>
-        <v>24460.5</v>
+        <v>29508.600000000002</v>
       </c>
     </row>
     <row r="56" spans="4:10" x14ac:dyDescent="0.25">
@@ -1845,22 +1845,22 @@
         <v>10000</v>
       </c>
       <c r="F56" s="1">
-        <v>24.171700000000001</v>
+        <v>30.018899999999999</v>
       </c>
       <c r="G56" s="1">
-        <v>24.146799999999999</v>
+        <v>29.9893</v>
       </c>
       <c r="H56" s="4">
         <f t="shared" si="10"/>
-        <v>0.99896986972368507</v>
+        <v>0.99901395454197195</v>
       </c>
       <c r="I56" s="7">
         <f t="shared" si="12"/>
-        <v>24171.7</v>
+        <v>30018.899999999998</v>
       </c>
       <c r="J56" s="7">
         <f t="shared" si="11"/>
-        <v>24146.799999999999</v>
+        <v>29989.3</v>
       </c>
     </row>
     <row r="57" spans="4:10" x14ac:dyDescent="0.25">
@@ -1871,22 +1871,22 @@
         <v>10000</v>
       </c>
       <c r="F57" s="1">
-        <v>23.453399999999998</v>
+        <v>29.299800000000001</v>
       </c>
       <c r="G57" s="1">
-        <v>23.438800000000001</v>
+        <v>29.269600000000001</v>
       </c>
       <c r="H57" s="4">
         <f t="shared" si="10"/>
-        <v>0.99937748897814394</v>
+        <v>0.99896927624079346</v>
       </c>
       <c r="I57" s="7">
         <f t="shared" si="12"/>
-        <v>23453.399999999998</v>
+        <v>29299.800000000003</v>
       </c>
       <c r="J57" s="7">
         <f t="shared" si="11"/>
-        <v>23438.799999999999</v>
+        <v>29269.600000000002</v>
       </c>
     </row>
     <row r="58" spans="4:10" x14ac:dyDescent="0.25">
@@ -1894,25 +1894,25 @@
         <v>46</v>
       </c>
       <c r="E58">
-        <v>10000</v>
+        <v>10016</v>
       </c>
       <c r="F58" s="1">
-        <v>22.456099999999999</v>
+        <v>28.265475239616599</v>
       </c>
       <c r="G58" s="1">
-        <v>22.4252</v>
+        <v>28.2357228434504</v>
       </c>
       <c r="H58" s="4">
         <f t="shared" si="10"/>
-        <v>0.99862398190246748</v>
+        <v>0.99894739444803327</v>
       </c>
       <c r="I58" s="7">
         <f t="shared" si="12"/>
-        <v>22456.1</v>
+        <v>28265.4752396166</v>
       </c>
       <c r="J58" s="7">
         <f t="shared" si="11"/>
-        <v>22425.200000000001</v>
+        <v>28235.7228434504</v>
       </c>
     </row>
     <row r="59" spans="4:10" x14ac:dyDescent="0.25">
@@ -1923,22 +1923,22 @@
         <v>10078</v>
       </c>
       <c r="F59" s="1">
-        <v>2.9554475094264698</v>
+        <v>3.4058344909704301</v>
       </c>
       <c r="G59" s="1">
-        <v>0.70043659456241303</v>
+        <v>1.0457432030164699</v>
       </c>
       <c r="H59" s="4">
         <f t="shared" si="10"/>
-        <v>0.23699848917240246</v>
+        <v>0.30704463349259953</v>
       </c>
       <c r="I59" s="6">
         <f t="shared" si="12"/>
-        <v>2955.4475094264699</v>
+        <v>3405.8344909704301</v>
       </c>
       <c r="J59" s="6">
         <f t="shared" si="11"/>
-        <v>700.43659456241301</v>
+        <v>1045.74320301647</v>
       </c>
     </row>
     <row r="60" spans="4:10" x14ac:dyDescent="0.25">
@@ -1949,22 +1949,22 @@
         <v>10000</v>
       </c>
       <c r="F60" s="1">
-        <v>24.8874</v>
+        <v>30.711200000000002</v>
       </c>
       <c r="G60" s="1">
-        <v>24.8597</v>
+        <v>30.683700000000002</v>
       </c>
       <c r="H60" s="4">
         <f t="shared" si="10"/>
-        <v>0.99888698698940026</v>
+        <v>0.99910456120242774</v>
       </c>
       <c r="I60" s="7">
         <f t="shared" si="12"/>
-        <v>24887.399999999998</v>
+        <v>30711.200000000001</v>
       </c>
       <c r="J60" s="7">
         <f t="shared" si="11"/>
-        <v>24859.7</v>
+        <v>30683.7</v>
       </c>
     </row>
     <row r="61" spans="4:10" x14ac:dyDescent="0.25">
@@ -1975,22 +1975,22 @@
         <v>10000</v>
       </c>
       <c r="F61" s="1">
-        <v>24.096800000000002</v>
+        <v>31.211200000000002</v>
       </c>
       <c r="G61" s="1">
-        <v>24.072800000000001</v>
+        <v>31.181000000000001</v>
       </c>
       <c r="H61" s="4">
         <f t="shared" si="10"/>
-        <v>0.99900401713090536</v>
+        <v>0.99903239862613413</v>
       </c>
       <c r="I61" s="5">
         <f t="shared" si="12"/>
-        <v>24096.800000000003</v>
+        <v>31211.200000000001</v>
       </c>
       <c r="J61" s="5">
         <f t="shared" si="11"/>
-        <v>24072.799999999999</v>
+        <v>31181</v>
       </c>
     </row>
     <row r="62" spans="4:10" x14ac:dyDescent="0.25">
@@ -2001,22 +2001,22 @@
         <v>10000</v>
       </c>
       <c r="F62" s="1">
-        <v>24.1386</v>
+        <v>30.390499999999999</v>
       </c>
       <c r="G62" s="1">
-        <v>24.1084</v>
+        <v>30.363199999999999</v>
       </c>
       <c r="H62" s="4">
         <f t="shared" si="10"/>
-        <v>0.99874889181642679</v>
+        <v>0.99910169296326157</v>
       </c>
       <c r="I62" s="7">
         <f t="shared" si="12"/>
-        <v>24138.6</v>
+        <v>30390.5</v>
       </c>
       <c r="J62" s="7">
         <f t="shared" si="11"/>
-        <v>24108.399999999998</v>
+        <v>30363.200000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>